<commit_message>
changes to run on docker
</commit_message>
<xml_diff>
--- a/src/test/resources/excel-data/TestData.xlsx
+++ b/src/test/resources/excel-data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IC0N\eclipse-workspace\Advanced Automation Framework Enterprise Level\src\test\resources\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9528BDE3-0AF0-4576-B4F0-3E61397F6126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A586A8-7678-42FA-852E-794A993F0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E664F8E6-5838-42F2-9B8D-5D11C748E4B3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>email</t>
   </si>
@@ -134,13 +134,19 @@
   </si>
   <si>
     <t>6576409789</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>120.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +158,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -530,7 +542,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5A7686-AF30-4FBB-ABD5-48A4A3008635}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K1" sqref="K1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,14 +614,15 @@
     <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -623,22 +636,25 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -652,22 +668,25 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -681,22 +700,25 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="I3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -710,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -722,10 +744,13 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -739,22 +764,25 @@
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -768,22 +796,25 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -797,29 +828,33 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{4B95BDC7-629E-4E1C-885D-DD90A92E82DF}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{9C3E82DB-BC2B-4829-8DCB-2F0D945EEC34}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{6A1B500E-1818-4804-8427-5CE05046DCDF}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{86DC9000-931D-4C12-A10E-C72E62D5F67F}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{1489E99C-0039-45A8-A26B-4A8F7DE67561}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{0BEF60EC-BD77-4797-8699-A35E381BB8C0}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{4B95BDC7-629E-4E1C-885D-DD90A92E82DF}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{9C3E82DB-BC2B-4829-8DCB-2F0D945EEC34}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{6A1B500E-1818-4804-8427-5CE05046DCDF}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{86DC9000-931D-4C12-A10E-C72E62D5F67F}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{1489E99C-0039-45A8-A26B-4A8F7DE67561}"/>
+    <hyperlink ref="H5" r:id="rId6" xr:uid="{0BEF60EC-BD77-4797-8699-A35E381BB8C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
configs and testdata changed to test the changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel-data/TestData.xlsx
+++ b/src/test/resources/excel-data/TestData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IC0N\eclipse-workspace\Advanced Automation Framework Enterprise Level\src\test\resources\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A586A8-7678-42FA-852E-794A993F0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FBA085-4FE9-40F9-9FDC-310282EAB500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E664F8E6-5838-42F2-9B8D-5D11C748E4B3}"/>
+    <workbookView xWindow="4950" yWindow="3300" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E664F8E6-5838-42F2-9B8D-5D11C748E4B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Manager" sheetId="2" r:id="rId1"/>
     <sheet name="LoginLogoutRegistration" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>email</t>
   </si>
@@ -124,22 +124,28 @@
     <t>LoginLogoutRegistration</t>
   </si>
   <si>
-    <t>Hamedani</t>
-  </si>
-  <si>
-    <t>Moshdada</t>
-  </si>
-  <si>
-    <t>moshdada.hamedani@example.com</t>
-  </si>
-  <si>
-    <t>6576409789</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
     <t>120.0</t>
+  </si>
+  <si>
+    <t>Boman</t>
+  </si>
+  <si>
+    <t>Irani</t>
+  </si>
+  <si>
+    <t>6576409987</t>
+  </si>
+  <si>
+    <t>boman.irani5@gmail.com</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>gdgd</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -605,7 +611,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:T1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -665,10 +671,10 @@
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
@@ -694,13 +700,13 @@
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -726,13 +732,13 @@
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -758,13 +764,13 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>5</v>
@@ -790,25 +796,25 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>3</v>
@@ -822,13 +828,13 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>14</v>

</xml_diff>